<commit_message>
Presentation and result table updated
</commit_message>
<xml_diff>
--- a/Text/ResultTable.xlsx
+++ b/Text/ResultTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\MasterWork\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CF4991-62A7-477D-9FCE-4EB547977206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DC7313-FECE-459B-89B0-0C417A79F005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28635" yWindow="-180" windowWidth="28740" windowHeight="15225" xr2:uid="{D3ADF6A4-700A-4A8A-9299-1DF2855E02F2}"/>
+    <workbookView xWindow="-28920" yWindow="-300" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D3ADF6A4-700A-4A8A-9299-1DF2855E02F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Day" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
   <si>
     <t>sand500</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>ARIMA(2,1,1)</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>ARIMA best</t>
   </si>
 </sst>
 </file>
@@ -505,17 +511,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438C3794-272D-434B-A315-715D3A0893A7}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -560,6 +566,9 @@
       <c r="E2">
         <v>3.4560102350031499</v>
       </c>
+      <c r="F2">
+        <v>5.3070760000000003</v>
+      </c>
       <c r="G2">
         <v>6.6079499999999998</v>
       </c>
@@ -586,6 +595,9 @@
       <c r="E3">
         <v>3.456715</v>
       </c>
+      <c r="F3">
+        <v>5.3028630000000003</v>
+      </c>
       <c r="G3">
         <v>6.6054620000000002</v>
       </c>
@@ -612,6 +624,9 @@
       <c r="E4">
         <v>3.9438469999999999</v>
       </c>
+      <c r="F4">
+        <v>5.7712870000000001</v>
+      </c>
       <c r="G4">
         <v>8.1828850000000006</v>
       </c>
@@ -638,6 +653,9 @@
       <c r="E5">
         <v>3.4810240000000001</v>
       </c>
+      <c r="F5">
+        <v>5.3930400000000001</v>
+      </c>
       <c r="G5">
         <v>6.6835990000000001</v>
       </c>
@@ -664,6 +682,9 @@
       <c r="E6">
         <v>3.4935849999999999</v>
       </c>
+      <c r="F6">
+        <v>5.4635090000000002</v>
+      </c>
       <c r="G6">
         <v>6.7389010000000003</v>
       </c>
@@ -678,8 +699,29 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
+      <c r="B7">
+        <v>3.572063</v>
+      </c>
+      <c r="C7">
+        <v>6.645429</v>
+      </c>
+      <c r="D7">
+        <v>7.6761410000000003</v>
+      </c>
+      <c r="E7">
+        <v>3.572063</v>
+      </c>
+      <c r="F7">
+        <v>5.303782</v>
+      </c>
       <c r="G7">
         <v>6.5509529999999998</v>
+      </c>
+      <c r="H7">
+        <v>8.5822479999999999</v>
+      </c>
+      <c r="I7">
+        <v>4.85473</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -796,6 +838,80 @@
       </c>
       <c r="I11">
         <v>1.9434214868225199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <f>MIN(B2:B11)</f>
+        <v>1.60611327054004</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:I14" si="0">MIN(C2:C11)</f>
+        <v>1.5979258462419501</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3.0947776926645498</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1.4551462465385601</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1.97049782277786</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.47287642938146</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>3.41975168038483</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>1.9434214868225199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <f>MIN(B2:B7)</f>
+        <v>3.572063</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:I15" si="1">MIN(C2:C7)</f>
+        <v>6.5213380000000001</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>7.551882</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>3.4560102350031499</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>5.3028630000000003</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>6.5509529999999998</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>8.2688729999999993</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>4.829968</v>
       </c>
     </row>
   </sheetData>
@@ -806,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011FE71D-ED27-4BB7-979B-21C8A9260921}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="A14" sqref="A14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,6 +977,9 @@
       <c r="E2">
         <v>3.5216820000000002</v>
       </c>
+      <c r="F2">
+        <v>5.3370759999999997</v>
+      </c>
       <c r="G2">
         <v>6.643459</v>
       </c>
@@ -887,6 +1006,9 @@
       <c r="E3">
         <v>3.8236349999999999</v>
       </c>
+      <c r="F3">
+        <v>5.8748690000000003</v>
+      </c>
       <c r="G3">
         <v>7.8076280000000002</v>
       </c>
@@ -913,6 +1035,9 @@
       <c r="E4">
         <v>3.5202089999999999</v>
       </c>
+      <c r="F4">
+        <v>5.795401</v>
+      </c>
       <c r="G4">
         <v>7.2528249999999996</v>
       </c>
@@ -939,6 +1064,9 @@
       <c r="E5">
         <v>4.0695259999999998</v>
       </c>
+      <c r="F5">
+        <v>5.8198460000000001</v>
+      </c>
       <c r="G5">
         <v>7.4388459999999998</v>
       </c>
@@ -965,6 +1093,9 @@
       <c r="E6">
         <v>3.5298970000000001</v>
       </c>
+      <c r="F6">
+        <v>5.4013210000000003</v>
+      </c>
       <c r="G6">
         <v>6.713317</v>
       </c>
@@ -991,6 +1122,9 @@
       <c r="E7">
         <v>3.5688810000000002</v>
       </c>
+      <c r="F7">
+        <v>5.4385820000000002</v>
+      </c>
       <c r="G7">
         <v>6.5287499999999996</v>
       </c>
@@ -1117,17 +1251,92 @@
         <v>6.1149021285508303</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <f>MIN(B2:B11)</f>
+        <v>3.7123153266168099</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:I14" si="0">MIN(C2:C11)</f>
+        <v>5.9871911782423499</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7.6684200000000002</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3.3309390789304998</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>5.0394440080612801</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>6.2694552903657197</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>8.3077883114687001</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>4.5120213352810499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <f>MIN(B2:B7)</f>
+        <v>3.8575469999999998</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:I15" si="1">MIN(C2:C7)</f>
+        <v>6.6105140000000002</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>7.6684200000000002</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>3.5202089999999999</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>5.3370759999999997</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>6.5287499999999996</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>8.4900529999999996</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>4.8883609999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEF0EC1-D25B-451E-97FE-CE691B0179BB}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1366,6 +1575,80 @@
         <v>5.4899114943475196</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <f>MIN(B2:B8)</f>
+        <v>4.5557610000000004</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:I14" si="0">MIN(C2:C8)</f>
+        <v>7.6615970000000004</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>9.4455256110775707</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4.1750790000000002</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>6.1475039999999996</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>7.3320540000000003</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>9.9920589999999994</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5.4899114943475196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <f>MIN(B2:B5)</f>
+        <v>4.5557610000000004</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:I15" si="1">MIN(C2:C5)</f>
+        <v>7.6615970000000004</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>9.5169049999999995</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>4.1750790000000002</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>6.1475039999999996</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>7.3320540000000003</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>9.9920589999999994</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>5.7332840000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1377,7 +1660,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>